<commit_message>
multi col vs col gen
</commit_message>
<xml_diff>
--- a/docs/Math3205 Project Formulation Comparison.xlsx
+++ b/docs/Math3205 Project Formulation Comparison.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xavie\Desktop\MATH3205_MPDPTW_Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1664816-54BC-4484-B276-DE1550C5DEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741FF3CF-E3E1-4D2E-A74F-CB6FD07E7B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{ABF29F5B-52A4-4B51-B67D-12561389EC32}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{ABF29F5B-52A4-4B51-B67D-12561389EC32}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
     <sheet name="Summary" sheetId="2" r:id="rId2"/>
+    <sheet name="Col Gen vs Multi Thread" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="185">
   <si>
     <t>Instance</t>
   </si>
@@ -587,6 +588,15 @@
   <si>
     <t>Col Gen</t>
   </si>
+  <si>
+    <t>Total Solved</t>
+  </si>
+  <si>
+    <t>Average By All</t>
+  </si>
+  <si>
+    <t>Multi Thread</t>
+  </si>
 </sst>
 </file>
 
@@ -609,7 +619,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -657,11 +667,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -680,6 +710,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1016,7 +1054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{120FBBEE-5035-451F-8043-D98BBCB1ED6E}">
   <dimension ref="B2:AP123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+    <sheetView zoomScale="93" workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
@@ -16200,14 +16238,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF0B8E3-04FC-42F8-B8DA-99369FD3F642}">
-  <dimension ref="C2:S27"/>
+  <dimension ref="C2:T29"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView zoomScale="69" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="3" max="3" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="11.90625" bestFit="1" customWidth="1"/>
@@ -16977,7 +17016,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="17" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C17" s="4" t="s">
         <v>164</v>
       </c>
@@ -17030,7 +17069,7 @@
         <v>3.8000000000000006E-2</v>
       </c>
     </row>
-    <row r="18" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C18" s="4" t="s">
         <v>165</v>
       </c>
@@ -17083,7 +17122,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="19" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C19" s="4" t="s">
         <v>166</v>
       </c>
@@ -17136,7 +17175,7 @@
         <v>0.36600000000000005</v>
       </c>
     </row>
-    <row r="20" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C20" s="4" t="s">
         <v>167</v>
       </c>
@@ -17189,7 +17228,7 @@
         <v>0.88800000000000012</v>
       </c>
     </row>
-    <row r="21" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C21" s="4" t="s">
         <v>168</v>
       </c>
@@ -17242,7 +17281,7 @@
         <v>12.492000000000001</v>
       </c>
     </row>
-    <row r="22" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C22" s="4" t="s">
         <v>169</v>
       </c>
@@ -17295,7 +17334,7 @@
         <v>77.067999999999998</v>
       </c>
     </row>
-    <row r="23" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C23" s="4" t="s">
         <v>170</v>
       </c>
@@ -17348,7 +17387,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C24" s="4" t="s">
         <v>171</v>
       </c>
@@ -17401,7 +17440,7 @@
         <v>0.192</v>
       </c>
     </row>
-    <row r="25" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C25" s="4" t="s">
         <v>172</v>
       </c>
@@ -17454,7 +17493,7 @@
         <v>0.34800000000000003</v>
       </c>
     </row>
-    <row r="26" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:20" x14ac:dyDescent="0.35">
       <c r="C26" s="4" t="s">
         <v>173</v>
       </c>
@@ -17507,57 +17546,986 @@
         <v>2.9059999999999997</v>
       </c>
     </row>
-    <row r="27" spans="3:19" x14ac:dyDescent="0.35">
-      <c r="C27" s="4" t="s">
+    <row r="27" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C27" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="D27" s="7">
-        <v>0</v>
-      </c>
-      <c r="E27" s="7">
+      <c r="D27" s="10">
+        <v>0</v>
+      </c>
+      <c r="E27" s="10">
         <v>57.668000000000006</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="H27" s="7">
-        <v>0</v>
-      </c>
-      <c r="I27" s="7">
+      <c r="H27" s="10">
+        <v>0</v>
+      </c>
+      <c r="I27" s="10">
         <v>55.227999999999994</v>
       </c>
-      <c r="J27" s="7" t="s">
+      <c r="J27" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="K27" s="8" t="s">
+      <c r="K27" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="L27" s="7">
-        <v>0</v>
-      </c>
-      <c r="M27" s="7">
+      <c r="L27" s="10">
+        <v>0</v>
+      </c>
+      <c r="M27" s="10">
         <v>47.696000000000005</v>
       </c>
-      <c r="N27" s="7" t="s">
+      <c r="N27" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="O27" s="8" t="s">
+      <c r="O27" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="P27" s="7">
+      <c r="P27" s="10">
         <v>5</v>
       </c>
-      <c r="Q27" s="7">
-        <v>0</v>
-      </c>
-      <c r="R27" s="7">
+      <c r="Q27" s="10">
+        <v>0</v>
+      </c>
+      <c r="R27" s="10">
         <v>128.024</v>
       </c>
-      <c r="S27" s="7">
+      <c r="S27" s="10">
         <v>60.019999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C28" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D28" s="7">
+        <f>SUM(D4:D27)</f>
+        <v>24</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H28" s="7">
+        <f>SUM(H4:H27)</f>
+        <v>40</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L28" s="7">
+        <f>SUM(L4:L27)</f>
+        <v>62</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="O28" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="P28" s="7">
+        <f>SUM(P4:P27)</f>
+        <v>114</v>
+      </c>
+      <c r="Q28" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="R28" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="S28" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="T28" s="7"/>
+    </row>
+    <row r="29" spans="3:20" x14ac:dyDescent="0.35">
+      <c r="C29" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="7">
+        <f>AVERAGE(E4:E27)</f>
+        <v>28.061250000000001</v>
+      </c>
+      <c r="F29" s="7">
+        <f t="shared" ref="F29:S29" si="0">AVERAGE(F4:F27)</f>
+        <v>217.79712500000002</v>
+      </c>
+      <c r="G29" s="8">
+        <f t="shared" si="0"/>
+        <v>85.436374999999998</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I29" s="7">
+        <f t="shared" si="0"/>
+        <v>22.264666666666667</v>
+      </c>
+      <c r="J29" s="7">
+        <f t="shared" si="0"/>
+        <v>328.25977272727272</v>
+      </c>
+      <c r="K29" s="8">
+        <f t="shared" si="0"/>
+        <v>224.73154545454551</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M29" s="7">
+        <f t="shared" si="0"/>
+        <v>15.341916666666664</v>
+      </c>
+      <c r="N29" s="7">
+        <f t="shared" si="0"/>
+        <v>117.61646666666667</v>
+      </c>
+      <c r="O29" s="8">
+        <f t="shared" si="0"/>
+        <v>106.74566666666668</v>
+      </c>
+      <c r="P29" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q29" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R29" s="7">
+        <f t="shared" si="0"/>
+        <v>44.211847826086967</v>
+      </c>
+      <c r="S29" s="7">
+        <f t="shared" si="0"/>
+        <v>22.31410869565217</v>
+      </c>
+      <c r="T29" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89BC1392-DE26-414E-B79B-3A7FB0BD29BA}">
+  <dimension ref="B2:H36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C2" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>15.06</v>
+      </c>
+      <c r="E4" s="4">
+        <v>31.3</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>21.54</v>
+      </c>
+      <c r="H4">
+        <v>11.45</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>11.06</v>
+      </c>
+      <c r="E5" s="4">
+        <v>21.58</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>13.76</v>
+      </c>
+      <c r="H5">
+        <v>12.73</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>5.09</v>
+      </c>
+      <c r="E6" s="4">
+        <v>13.88</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>5.24</v>
+      </c>
+      <c r="H6">
+        <v>9.68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>6.26</v>
+      </c>
+      <c r="E7" s="4">
+        <v>13.8</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>6.58</v>
+      </c>
+      <c r="H7">
+        <v>7.34</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>113.5</v>
+      </c>
+      <c r="E8" s="4">
+        <v>251.76</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>145.09</v>
+      </c>
+      <c r="H8">
+        <v>143.84</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>3135.85</v>
+      </c>
+      <c r="H9">
+        <v>843.25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>123.9</v>
+      </c>
+      <c r="E10" s="4">
+        <v>230.77</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>194.13</v>
+      </c>
+      <c r="H10">
+        <v>96.1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>632.54999999999995</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1166.6500000000001</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1147.6300000000001</v>
+      </c>
+      <c r="H11">
+        <v>485.64</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>450.38</v>
+      </c>
+      <c r="E12" s="4">
+        <v>791.43</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>836.67</v>
+      </c>
+      <c r="H12">
+        <v>318.62</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0.44</v>
+      </c>
+      <c r="E13" s="4">
+        <v>6.13</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0.44</v>
+      </c>
+      <c r="H13">
+        <v>6.62</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="E14" s="4">
+        <v>62.44</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>21.72</v>
+      </c>
+      <c r="H14">
+        <v>49.66</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>3.68</v>
+      </c>
+      <c r="E15" s="4">
+        <v>10.51</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>3.68</v>
+      </c>
+      <c r="H15">
+        <v>11.04</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>2.25</v>
+      </c>
+      <c r="E16" s="4">
+        <v>15.06</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>2.27</v>
+      </c>
+      <c r="H16">
+        <v>17.18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>6.6</v>
+      </c>
+      <c r="E17" s="4">
+        <v>23.3</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>6.7</v>
+      </c>
+      <c r="H17">
+        <v>23.92</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1.04</v>
+      </c>
+      <c r="E18" s="4">
+        <v>2.91</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1.03</v>
+      </c>
+      <c r="H18">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>7.42</v>
+      </c>
+      <c r="E19" s="4">
+        <v>19.38</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>7.6</v>
+      </c>
+      <c r="H19">
+        <v>9.73</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>18.37</v>
+      </c>
+      <c r="E20" s="4">
+        <v>41.18</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>20.37</v>
+      </c>
+      <c r="H20">
+        <v>14.48</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B21" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>15.92</v>
+      </c>
+      <c r="E21" s="4">
+        <v>32.35</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>23.64</v>
+      </c>
+      <c r="H21">
+        <v>13.22</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B22" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>12.86</v>
+      </c>
+      <c r="E22" s="4">
+        <v>30.38</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>18.3</v>
+      </c>
+      <c r="H22">
+        <v>10.93</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B23" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>7.89</v>
+      </c>
+      <c r="E23" s="4">
+        <v>18.05</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>8.77</v>
+      </c>
+      <c r="H23">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B24" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>53.15</v>
+      </c>
+      <c r="E24" s="4">
+        <v>114.16</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>58.31</v>
+      </c>
+      <c r="H24">
+        <v>43.31</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B25" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>113.64</v>
+      </c>
+      <c r="E25" s="4">
+        <v>218.54</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>305.44</v>
+      </c>
+      <c r="H25">
+        <v>100.82</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B26" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>23.23</v>
+      </c>
+      <c r="E26" s="4">
+        <v>59.52</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>25.11</v>
+      </c>
+      <c r="H26">
+        <v>22.58</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B27" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>145.49</v>
+      </c>
+      <c r="E27" s="4">
+        <v>329.67</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>154.69</v>
+      </c>
+      <c r="H27">
+        <v>101.22</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B28" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>49.83</v>
+      </c>
+      <c r="E28" s="4">
+        <v>111.73</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>62.45</v>
+      </c>
+      <c r="H28">
+        <v>35.1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B29" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1251.8900000000001</v>
+      </c>
+      <c r="H29">
+        <v>1554.7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B30" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>3.48</v>
+      </c>
+      <c r="E30" s="4">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>4.42</v>
+      </c>
+      <c r="H30">
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B31" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>4.42</v>
+      </c>
+      <c r="E31" s="4">
+        <v>9.74</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>4.72</v>
+      </c>
+      <c r="H31">
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B32" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>89.35</v>
+      </c>
+      <c r="E32" s="4">
+        <v>187.07</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>119.82</v>
+      </c>
+      <c r="H32">
+        <v>132.19</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B33" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>20.02</v>
+      </c>
+      <c r="E33" s="4">
+        <v>43.25</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>26.07</v>
+      </c>
+      <c r="H33">
+        <v>30.49</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B34" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>23.19</v>
+      </c>
+      <c r="E34" s="4">
+        <v>53.42</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>30.13</v>
+      </c>
+      <c r="H34">
+        <v>50.26</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B35" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>87.83</v>
+      </c>
+      <c r="E35" s="4">
+        <v>188.59</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>106.94</v>
+      </c>
+      <c r="H35">
+        <v>164.88</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B36" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>79.709999999999994</v>
+      </c>
+      <c r="E36" s="4">
+        <v>167.79</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>105.14</v>
+      </c>
+      <c r="H36">
+        <v>106.49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>